<commit_message>
Fix a bug where (experimental) long format code interfered with (traditional) wide format code
</commit_message>
<xml_diff>
--- a/tests/scores.xlsx
+++ b/tests/scores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debrouwere/Documents/Research/packages/brr/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95E2B50A-E2C7-9747-ADFB-120605DCB6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BC6353-B481-E748-9795-A01FFAAA716F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26800" xr2:uid="{2188AE81-7497-FF43-A1A7-730F826C481F}"/>
   </bookViews>
@@ -158,9 +158,6 @@
     <t>error</t>
   </si>
   <si>
-    <t>assessment</t>
-  </si>
-  <si>
     <t>domain</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>scie</t>
+  </si>
+  <si>
+    <t>cycle</t>
   </si>
 </sst>
 </file>
@@ -178,7 +178,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="#,##0.00000000000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00000000000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -273,12 +273,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -619,7 +619,7 @@
   <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,10 +630,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>37</v>
@@ -650,7 +650,7 @@
         <v>2022</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -667,7 +667,7 @@
         <v>2022</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -684,7 +684,7 @@
         <v>2022</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -701,7 +701,7 @@
         <v>2022</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
@@ -718,7 +718,7 @@
         <v>2022</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>
@@ -735,7 +735,7 @@
         <v>2022</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -752,7 +752,7 @@
         <v>2022</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -769,7 +769,7 @@
         <v>2022</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -786,7 +786,7 @@
         <v>2022</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>8</v>
@@ -803,7 +803,7 @@
         <v>2022</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>9</v>
@@ -820,7 +820,7 @@
         <v>2022</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>10</v>
@@ -837,7 +837,7 @@
         <v>2022</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
@@ -854,7 +854,7 @@
         <v>2022</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>12</v>
@@ -871,7 +871,7 @@
         <v>2022</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
@@ -888,7 +888,7 @@
         <v>2022</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>14</v>
@@ -905,7 +905,7 @@
         <v>2022</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>15</v>
@@ -922,7 +922,7 @@
         <v>2022</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>16</v>
@@ -939,7 +939,7 @@
         <v>2022</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>17</v>
@@ -956,7 +956,7 @@
         <v>2022</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>18</v>
@@ -973,7 +973,7 @@
         <v>2022</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>19</v>
@@ -990,7 +990,7 @@
         <v>2022</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>20</v>
@@ -1007,7 +1007,7 @@
         <v>2022</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>21</v>
@@ -1024,7 +1024,7 @@
         <v>2022</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>22</v>
@@ -1041,7 +1041,7 @@
         <v>2022</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>23</v>
@@ -1058,7 +1058,7 @@
         <v>2022</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>24</v>
@@ -1075,7 +1075,7 @@
         <v>2022</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>25</v>
@@ -1092,7 +1092,7 @@
         <v>2022</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>26</v>
@@ -1109,7 +1109,7 @@
         <v>2022</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>27</v>
@@ -1126,7 +1126,7 @@
         <v>2022</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>28</v>
@@ -1143,7 +1143,7 @@
         <v>2022</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>29</v>
@@ -1160,7 +1160,7 @@
         <v>2022</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>30</v>
@@ -1177,7 +1177,7 @@
         <v>2022</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>31</v>
@@ -1194,7 +1194,7 @@
         <v>2022</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>32</v>
@@ -1211,7 +1211,7 @@
         <v>2022</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>33</v>
@@ -1228,7 +1228,7 @@
         <v>2022</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>34</v>
@@ -1245,7 +1245,7 @@
         <v>2022</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>35</v>
@@ -1262,7 +1262,7 @@
         <v>2022</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>36</v>
@@ -1279,7 +1279,7 @@
         <v>2022</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>0</v>
@@ -1296,7 +1296,7 @@
         <v>2022</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>1</v>
@@ -1313,7 +1313,7 @@
         <v>2022</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>2</v>
@@ -1330,7 +1330,7 @@
         <v>2022</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>3</v>
@@ -1347,7 +1347,7 @@
         <v>2022</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>4</v>
@@ -1364,7 +1364,7 @@
         <v>2022</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>5</v>
@@ -1381,7 +1381,7 @@
         <v>2022</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>6</v>
@@ -1398,7 +1398,7 @@
         <v>2022</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>7</v>
@@ -1415,7 +1415,7 @@
         <v>2022</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>8</v>
@@ -1432,7 +1432,7 @@
         <v>2022</v>
       </c>
       <c r="B48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>9</v>
@@ -1449,7 +1449,7 @@
         <v>2022</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>10</v>
@@ -1466,7 +1466,7 @@
         <v>2022</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>11</v>
@@ -1483,7 +1483,7 @@
         <v>2022</v>
       </c>
       <c r="B51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>12</v>
@@ -1500,7 +1500,7 @@
         <v>2022</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>13</v>
@@ -1517,7 +1517,7 @@
         <v>2022</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>14</v>
@@ -1534,7 +1534,7 @@
         <v>2022</v>
       </c>
       <c r="B54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>15</v>
@@ -1551,7 +1551,7 @@
         <v>2022</v>
       </c>
       <c r="B55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>16</v>
@@ -1568,7 +1568,7 @@
         <v>2022</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>17</v>
@@ -1585,7 +1585,7 @@
         <v>2022</v>
       </c>
       <c r="B57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>18</v>
@@ -1602,7 +1602,7 @@
         <v>2022</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>19</v>
@@ -1619,7 +1619,7 @@
         <v>2022</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>20</v>
@@ -1636,7 +1636,7 @@
         <v>2022</v>
       </c>
       <c r="B60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>21</v>
@@ -1653,7 +1653,7 @@
         <v>2022</v>
       </c>
       <c r="B61" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>22</v>
@@ -1670,7 +1670,7 @@
         <v>2022</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>23</v>
@@ -1687,7 +1687,7 @@
         <v>2022</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>24</v>
@@ -1704,7 +1704,7 @@
         <v>2022</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>25</v>
@@ -1721,7 +1721,7 @@
         <v>2022</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>26</v>
@@ -1738,7 +1738,7 @@
         <v>2022</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>27</v>
@@ -1755,7 +1755,7 @@
         <v>2022</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>28</v>
@@ -1772,7 +1772,7 @@
         <v>2022</v>
       </c>
       <c r="B68" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>29</v>
@@ -1789,7 +1789,7 @@
         <v>2022</v>
       </c>
       <c r="B69" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>30</v>
@@ -1806,7 +1806,7 @@
         <v>2022</v>
       </c>
       <c r="B70" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>31</v>
@@ -1823,7 +1823,7 @@
         <v>2022</v>
       </c>
       <c r="B71" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>32</v>
@@ -1840,7 +1840,7 @@
         <v>2022</v>
       </c>
       <c r="B72" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>33</v>
@@ -1857,7 +1857,7 @@
         <v>2022</v>
       </c>
       <c r="B73" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>34</v>
@@ -1874,7 +1874,7 @@
         <v>2022</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>35</v>
@@ -1891,7 +1891,7 @@
         <v>2022</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>36</v>
@@ -1908,7 +1908,7 @@
         <v>2022</v>
       </c>
       <c r="B76" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>0</v>
@@ -1925,7 +1925,7 @@
         <v>2022</v>
       </c>
       <c r="B77" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>1</v>
@@ -1942,7 +1942,7 @@
         <v>2022</v>
       </c>
       <c r="B78" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>2</v>
@@ -1959,7 +1959,7 @@
         <v>2022</v>
       </c>
       <c r="B79" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>3</v>
@@ -1976,7 +1976,7 @@
         <v>2022</v>
       </c>
       <c r="B80" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>4</v>
@@ -1993,7 +1993,7 @@
         <v>2022</v>
       </c>
       <c r="B81" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>5</v>
@@ -2010,7 +2010,7 @@
         <v>2022</v>
       </c>
       <c r="B82" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>6</v>
@@ -2027,7 +2027,7 @@
         <v>2022</v>
       </c>
       <c r="B83" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>7</v>
@@ -2044,7 +2044,7 @@
         <v>2022</v>
       </c>
       <c r="B84" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>8</v>
@@ -2061,7 +2061,7 @@
         <v>2022</v>
       </c>
       <c r="B85" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>9</v>
@@ -2078,7 +2078,7 @@
         <v>2022</v>
       </c>
       <c r="B86" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>10</v>
@@ -2095,7 +2095,7 @@
         <v>2022</v>
       </c>
       <c r="B87" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>11</v>
@@ -2112,7 +2112,7 @@
         <v>2022</v>
       </c>
       <c r="B88" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>12</v>
@@ -2129,7 +2129,7 @@
         <v>2022</v>
       </c>
       <c r="B89" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>13</v>
@@ -2146,7 +2146,7 @@
         <v>2022</v>
       </c>
       <c r="B90" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>14</v>
@@ -2163,7 +2163,7 @@
         <v>2022</v>
       </c>
       <c r="B91" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>15</v>
@@ -2180,7 +2180,7 @@
         <v>2022</v>
       </c>
       <c r="B92" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>16</v>
@@ -2197,7 +2197,7 @@
         <v>2022</v>
       </c>
       <c r="B93" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>17</v>
@@ -2214,7 +2214,7 @@
         <v>2022</v>
       </c>
       <c r="B94" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>18</v>
@@ -2231,7 +2231,7 @@
         <v>2022</v>
       </c>
       <c r="B95" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>19</v>
@@ -2248,7 +2248,7 @@
         <v>2022</v>
       </c>
       <c r="B96" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>20</v>
@@ -2265,7 +2265,7 @@
         <v>2022</v>
       </c>
       <c r="B97" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>21</v>
@@ -2282,7 +2282,7 @@
         <v>2022</v>
       </c>
       <c r="B98" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>22</v>
@@ -2299,7 +2299,7 @@
         <v>2022</v>
       </c>
       <c r="B99" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>23</v>
@@ -2316,7 +2316,7 @@
         <v>2022</v>
       </c>
       <c r="B100" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>24</v>
@@ -2333,7 +2333,7 @@
         <v>2022</v>
       </c>
       <c r="B101" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>25</v>
@@ -2350,7 +2350,7 @@
         <v>2022</v>
       </c>
       <c r="B102" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>26</v>
@@ -2367,7 +2367,7 @@
         <v>2022</v>
       </c>
       <c r="B103" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>27</v>
@@ -2384,7 +2384,7 @@
         <v>2022</v>
       </c>
       <c r="B104" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>28</v>
@@ -2401,7 +2401,7 @@
         <v>2022</v>
       </c>
       <c r="B105" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>29</v>
@@ -2418,7 +2418,7 @@
         <v>2022</v>
       </c>
       <c r="B106" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>30</v>
@@ -2435,7 +2435,7 @@
         <v>2022</v>
       </c>
       <c r="B107" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>31</v>
@@ -2452,7 +2452,7 @@
         <v>2022</v>
       </c>
       <c r="B108" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>32</v>
@@ -2469,7 +2469,7 @@
         <v>2022</v>
       </c>
       <c r="B109" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>33</v>
@@ -2486,7 +2486,7 @@
         <v>2022</v>
       </c>
       <c r="B110" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>34</v>
@@ -2503,7 +2503,7 @@
         <v>2022</v>
       </c>
       <c r="B111" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>35</v>
@@ -2520,7 +2520,7 @@
         <v>2022</v>
       </c>
       <c r="B112" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>36</v>

</xml_diff>